<commit_message>
Init Adjacency via List works !!!
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>LoadNodes und LoadTriangles in eine Funktion</t>
+    <t>Wahl des Nachbardreiecks in Promenade</t>
   </si>
   <si>
-    <t>Map Ansatz</t>
+    <t>Visualisierung -&gt; Pfad in Maillage</t>
   </si>
   <si>
-    <t>Listen Ansatz</t>
+    <t>Listen Ansatz (sort)</t>
   </si>
   <si>
-    <t>Visualisierung</t>
+    <t>Laufzeit / Komplexität</t>
   </si>
   <si>
-    <t>MakeFile</t>
+    <t>Promenade falls kein Nachbar existiert (-1)</t>
   </si>
 </sst>
 </file>
@@ -390,24 +390,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:B13"/>
+  <dimension ref="B9:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>2</v>
@@ -415,11 +405,21 @@
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Promenade mit aire und min_neg funktioniert :D
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Wahl des Nachbardreiecks in Promenade</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Promenade falls kein Nachbar existiert (-1)</t>
+  </si>
+  <si>
+    <t>Latex akzente</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B9:B17"/>
+  <dimension ref="B9:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -423,6 +426,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Blank space in Terminal Output removed
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Wahl des Nachbardreiecks in Promenade</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>Latex akzente</t>
+  </si>
+  <si>
+    <t>Aufgabe 5 Rekurrenz</t>
+  </si>
+  <si>
+    <t>Random Neighbor selection</t>
   </si>
 </sst>
 </file>
@@ -393,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B9:B19"/>
+  <dimension ref="B9:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -431,6 +437,16 @@
         <v>5</v>
       </c>
     </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
time measurement adj meth
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Laufzeit / Komplexität</t>
   </si>
@@ -35,13 +35,7 @@
     <t>anderes Maillage</t>
   </si>
   <si>
-    <t>Testdatei in Main (Nachbarschaft, Prom, covering Tri)</t>
-  </si>
-  <si>
     <t>Vergleich random und min_neg: Datei mit Testpunkten und Startdreiecken, Plots speichern, Pfadlänge, Zeit, ganz feines Mesh für Zeitvergleich</t>
-  </si>
-  <si>
-    <t>code aufräumen und kommentieren</t>
   </si>
 </sst>
 </file>
@@ -396,7 +390,7 @@
   <dimension ref="B3:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -411,19 +405,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.45">

</xml_diff>